<commit_message>
Ajuste na validação com Pandera
</commit_message>
<xml_diff>
--- a/data/raw/base.xlsx
+++ b/data/raw/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\VS_Code\Projetos e Estudos\- PROCESSO SELETIVO - PREPARAÇÃO\12. Cases Técnicos\case_gb\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0F8E62-C17E-48C5-8437-D7B8E9155BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5499EEB5-DFA0-4428-8556-61DD722824E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16084" uniqueCount="2623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16084" uniqueCount="2624">
   <si>
     <t>DT_MES</t>
   </si>
@@ -7909,6 +7909,9 @@
   </si>
   <si>
     <t>AC</t>
+  </si>
+  <si>
+    <t>dfg</t>
   </si>
 </sst>
 </file>
@@ -45770,7 +45773,7 @@
     <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2571</v>
       </c>
@@ -45799,7 +45802,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45828,7 +45831,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45857,7 +45860,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45886,7 +45889,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45915,7 +45918,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45944,7 +45947,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45973,7 +45976,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46002,7 +46005,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46031,7 +46034,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46060,7 +46063,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46089,7 +46092,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46118,7 +46121,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46147,7 +46150,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46176,7 +46179,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46205,7 +46208,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46234,7 +46237,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46263,7 +46266,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46292,7 +46295,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46321,7 +46324,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46350,7 +46353,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46379,7 +46382,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46408,7 +46411,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46437,7 +46440,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46466,7 +46469,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46495,7 +46498,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46524,7 +46527,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46553,7 +46556,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46582,7 +46585,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46611,7 +46614,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46640,7 +46643,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46669,7 +46672,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46698,7 +46701,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46727,7 +46730,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46756,7 +46759,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46785,7 +46788,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46814,7 +46817,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46843,7 +46846,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46872,7 +46875,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46901,7 +46904,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46930,7 +46933,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2579</v>
       </c>
@@ -86324,16 +86327,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -86353,7 +86356,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>202102</v>
       </c>
@@ -86373,7 +86376,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>202101</v>
       </c>
@@ -86393,7 +86396,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>202104</v>
       </c>
@@ -86413,7 +86416,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>202106</v>
       </c>
@@ -86433,7 +86436,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>202103</v>
       </c>
@@ -86453,7 +86456,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>202105</v>
       </c>
@@ -86473,7 +86476,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>202107</v>
       </c>
@@ -86493,7 +86496,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>202108</v>
       </c>
@@ -86513,7 +86516,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>202106</v>
       </c>
@@ -86530,10 +86533,10 @@
         <v>2600</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>2601</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>202105</v>
       </c>
@@ -86553,7 +86556,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>202102</v>
       </c>
@@ -86572,8 +86575,9 @@
       <c r="F12" s="1" t="s">
         <v>2601</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>202107</v>
       </c>
@@ -86593,7 +86597,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>202108</v>
       </c>
@@ -86613,7 +86617,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>202101</v>
       </c>
@@ -86633,7 +86637,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>202103</v>
       </c>
@@ -86653,7 +86657,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>202104</v>
       </c>
@@ -86673,7 +86677,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>202105</v>
       </c>
@@ -86693,7 +86697,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>202108</v>
       </c>
@@ -86713,7 +86717,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>202102</v>
       </c>
@@ -86733,7 +86737,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>202103</v>
       </c>
@@ -86753,7 +86757,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>202101</v>
       </c>
@@ -86773,7 +86777,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>202106</v>
       </c>
@@ -86793,7 +86797,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>202104</v>
       </c>
@@ -86813,7 +86817,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>202107</v>
       </c>
@@ -86833,7 +86837,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>202103</v>
       </c>
@@ -86853,7 +86857,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>202105</v>
       </c>
@@ -86873,7 +86877,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>202107</v>
       </c>
@@ -86893,7 +86897,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>202101</v>
       </c>
@@ -86913,7 +86917,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>202106</v>
       </c>
@@ -86933,7 +86937,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>202102</v>
       </c>
@@ -86953,7 +86957,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>202104</v>
       </c>
@@ -86973,7 +86977,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>202108</v>
       </c>
@@ -86993,7 +86997,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>202107</v>
       </c>
@@ -87013,7 +87017,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>202108</v>
       </c>
@@ -87033,7 +87037,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>202101</v>
       </c>
@@ -87053,7 +87057,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>202105</v>
       </c>
@@ -87073,7 +87077,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>202106</v>
       </c>
@@ -87093,7 +87097,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>202103</v>
       </c>
@@ -87113,7 +87117,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>202102</v>
       </c>
@@ -87133,7 +87137,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>202104</v>
       </c>

</xml_diff>